<commit_message>
Remove hydrography from data file
</commit_message>
<xml_diff>
--- a/pyrite_data.xlsx
+++ b/pyrite_data.xlsx
@@ -8,21 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vamaral/GoogleDrive/DOCS/Py_work/pyEXPORTS/pyrite_dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF57C27D-C420-8743-ABE1-13E4D93C891C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703AAB89-39D8-2549-9FD1-E99F2C442F26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" activeTab="5" xr2:uid="{2E5AD777-6D2C-6A4D-B8DC-BC8EB3802093}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" xr2:uid="{2E5AD777-6D2C-6A4D-B8DC-BC8EB3802093}"/>
   </bookViews>
   <sheets>
-    <sheet name="hydrography" sheetId="1" r:id="rId1"/>
-    <sheet name="POC" sheetId="3" r:id="rId2"/>
-    <sheet name="Ti" sheetId="9" r:id="rId3"/>
-    <sheet name="Ti_w_OL" sheetId="10" r:id="rId4"/>
-    <sheet name="NPP" sheetId="4" r:id="rId5"/>
-    <sheet name="POC_fluxes_thorium" sheetId="6" r:id="rId6"/>
-    <sheet name="POC_fluxes_traps" sheetId="7" r:id="rId7"/>
+    <sheet name="POC" sheetId="3" r:id="rId1"/>
+    <sheet name="Ti" sheetId="9" r:id="rId2"/>
+    <sheet name="Ti_w_OL" sheetId="10" r:id="rId3"/>
+    <sheet name="NPP" sheetId="4" r:id="rId4"/>
+    <sheet name="POC_fluxes_thorium" sheetId="6" r:id="rId5"/>
+    <sheet name="POC_fluxes_traps" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Ti!$A$1:$E$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Ti!$A$1:$E$66</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,18 +42,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="24">
   <si>
     <t>depth</t>
-  </si>
-  <si>
-    <t>t_c</t>
-  </si>
-  <si>
-    <t>s_psu</t>
-  </si>
-  <si>
-    <t>sigT_kgpmc</t>
   </si>
   <si>
     <t>pump_cast</t>
@@ -482,223 +472,1135 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFBBAFA-EF7D-7549-B349-DBECFE07DC79}">
-  <dimension ref="A1:D15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE25169-79B8-4E46-8D5E-6F3E6298BD3C}">
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>0.89018926324458014</v>
+      </c>
+      <c r="E2">
+        <v>5.1705846886633579E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>95</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>0.7153182801862531</v>
+      </c>
+      <c r="E3">
+        <v>5.6390084453433444E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>145</v>
+      </c>
+      <c r="C4">
+        <v>150</v>
+      </c>
+      <c r="D4">
+        <v>0.45001749959423903</v>
+      </c>
+      <c r="E4">
+        <v>2.9521695366396945E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>195</v>
+      </c>
+      <c r="C5">
+        <v>200</v>
+      </c>
+      <c r="D5">
+        <v>0.32799509976152702</v>
+      </c>
+      <c r="E5">
+        <v>3.3186393281012902E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>330</v>
+      </c>
+      <c r="C6">
+        <v>330</v>
+      </c>
+      <c r="D6">
+        <v>0.23470265158527037</v>
+      </c>
+      <c r="E6">
+        <v>1.3346149733508459E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>500</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="D7">
+        <v>0.16060151501673745</v>
+      </c>
+      <c r="E7">
+        <v>2.9017651343523899E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>95</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>0.76714065045124069</v>
+      </c>
+      <c r="E8">
+        <v>6.7528084284768516E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>145</v>
+      </c>
+      <c r="C9">
+        <v>150</v>
+      </c>
+      <c r="D9">
+        <v>0.45829556808001809</v>
+      </c>
+      <c r="E9">
+        <v>5.4768237017384015E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>195</v>
+      </c>
+      <c r="C10">
+        <v>200</v>
+      </c>
+      <c r="D10">
+        <v>0.36324594343047573</v>
+      </c>
+      <c r="E10">
+        <v>8.6819214292885818E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>330</v>
+      </c>
+      <c r="C11">
+        <v>330</v>
+      </c>
+      <c r="D11">
+        <v>0.26489067375352698</v>
+      </c>
+      <c r="E11">
+        <v>4.7020009797597462E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>500</v>
+      </c>
+      <c r="C12">
+        <v>500</v>
+      </c>
+      <c r="D12">
+        <v>0.17589614981315357</v>
+      </c>
+      <c r="E12">
+        <v>3.0020056295142577E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>502.94</v>
-      </c>
-      <c r="B2">
-        <v>3.9184999999999999</v>
-      </c>
-      <c r="C2">
-        <v>34.095999999999997</v>
-      </c>
-      <c r="D2">
-        <v>27.078900000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>502.20800000000003</v>
-      </c>
-      <c r="B3">
-        <v>3.9142000000000001</v>
-      </c>
-      <c r="C3">
-        <v>34.0959</v>
-      </c>
-      <c r="D3">
-        <v>27.0793</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>333.20800000000003</v>
-      </c>
-      <c r="B4">
-        <v>4.2389999999999999</v>
-      </c>
-      <c r="C4">
-        <v>33.917200000000001</v>
-      </c>
-      <c r="D4">
-        <v>26.9026</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>198.334</v>
-      </c>
-      <c r="B5">
-        <v>4.7153</v>
-      </c>
-      <c r="C5">
-        <v>33.738100000000003</v>
-      </c>
-      <c r="D5">
-        <v>26.708300000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>149.476</v>
-      </c>
-      <c r="B6">
-        <v>5.117</v>
-      </c>
-      <c r="C6">
-        <v>33.635599999999997</v>
-      </c>
-      <c r="D6">
-        <v>26.581600000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>122.679</v>
-      </c>
-      <c r="B7">
-        <v>5.2005999999999997</v>
-      </c>
-      <c r="C7">
-        <v>33.300699999999999</v>
-      </c>
-      <c r="D7">
-        <v>26.3065</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>108.366</v>
-      </c>
-      <c r="B8">
-        <v>5.7461000000000002</v>
-      </c>
-      <c r="C8">
-        <v>32.875300000000003</v>
-      </c>
-      <c r="D8">
-        <v>25.905799999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>98.396000000000001</v>
-      </c>
-      <c r="B9">
-        <v>5.6346999999999996</v>
-      </c>
-      <c r="C9">
-        <v>32.657899999999998</v>
-      </c>
-      <c r="D9">
-        <v>25.7471</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>79.132999999999996</v>
-      </c>
-      <c r="B10">
-        <v>6.4250999999999996</v>
-      </c>
-      <c r="C10">
-        <v>32.532699999999998</v>
-      </c>
-      <c r="D10">
-        <v>25.551300000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>63.323</v>
-      </c>
-      <c r="B11">
-        <v>7.0972</v>
-      </c>
-      <c r="C11">
-        <v>32.489100000000001</v>
-      </c>
-      <c r="D11">
-        <v>25.429099999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>48.487000000000002</v>
-      </c>
-      <c r="B12">
-        <v>9.1615000000000002</v>
-      </c>
-      <c r="C12">
-        <v>32.426900000000003</v>
-      </c>
-      <c r="D12">
-        <v>25.0794</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>34.249000000000002</v>
-      </c>
       <c r="B13">
-        <v>13.8917</v>
+        <v>50</v>
       </c>
       <c r="C13">
-        <v>32.319099999999999</v>
+        <v>50</v>
       </c>
       <c r="D13">
-        <v>24.139299999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1.2689791897719822</v>
+      </c>
+      <c r="E13">
+        <v>4.5664085135654703E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>20.795999999999999</v>
+        <v>3</v>
       </c>
       <c r="B14">
-        <v>14.0215</v>
+        <v>95</v>
       </c>
       <c r="C14">
-        <v>32.3155</v>
+        <v>100</v>
       </c>
       <c r="D14">
-        <v>24.109500000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.60800985133817231</v>
+      </c>
+      <c r="E14">
+        <v>3.1485506684334891E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>5.2409999999999997</v>
+        <v>3</v>
       </c>
       <c r="B15">
-        <v>14.0283</v>
+        <v>330</v>
       </c>
       <c r="C15">
-        <v>32.313899999999997</v>
+        <v>330</v>
       </c>
       <c r="D15">
-        <v>24.1065</v>
+        <v>0.2316044991594198</v>
+      </c>
+      <c r="E15">
+        <v>3.28077591613158E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>500</v>
+      </c>
+      <c r="C16">
+        <v>500</v>
+      </c>
+      <c r="D16">
+        <v>0.16308334946888314</v>
+      </c>
+      <c r="E16">
+        <v>2.8194862359707629E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>50</v>
+      </c>
+      <c r="C17">
+        <v>50</v>
+      </c>
+      <c r="D17">
+        <v>1.9210846893753761</v>
+      </c>
+      <c r="E17">
+        <v>5.629286089011809E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>95</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+      <c r="D18">
+        <v>0.68365844702112921</v>
+      </c>
+      <c r="E18">
+        <v>3.0527088383164643E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>145</v>
+      </c>
+      <c r="C19">
+        <v>150</v>
+      </c>
+      <c r="D19">
+        <v>0.30309983851927552</v>
+      </c>
+      <c r="E19">
+        <v>1.4723993683688132E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>195</v>
+      </c>
+      <c r="C20">
+        <v>200</v>
+      </c>
+      <c r="D20">
+        <v>0.20886446167605854</v>
+      </c>
+      <c r="E20">
+        <v>3.3939938719133519E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>330</v>
+      </c>
+      <c r="C21">
+        <v>330</v>
+      </c>
+      <c r="D21">
+        <v>0.23590323149316275</v>
+      </c>
+      <c r="E21">
+        <v>4.7415563866089437E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>500</v>
+      </c>
+      <c r="C22">
+        <v>500</v>
+      </c>
+      <c r="D22">
+        <v>0.14285656260224014</v>
+      </c>
+      <c r="E22">
+        <v>3.0217055848894739E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>50</v>
+      </c>
+      <c r="C23">
+        <v>50</v>
+      </c>
+      <c r="D23">
+        <v>1.0748191044702937</v>
+      </c>
+      <c r="E23">
+        <v>2.5844200517237025E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>95</v>
+      </c>
+      <c r="C24">
+        <v>100</v>
+      </c>
+      <c r="D24">
+        <v>0.61992127892280602</v>
+      </c>
+      <c r="E24">
+        <v>1.5874341595665566E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>145</v>
+      </c>
+      <c r="C25">
+        <v>150</v>
+      </c>
+      <c r="D25">
+        <v>0.35753418573162649</v>
+      </c>
+      <c r="E25">
+        <v>2.260660010593386E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>330</v>
+      </c>
+      <c r="C26">
+        <v>330</v>
+      </c>
+      <c r="D26">
+        <v>0.26901829959445928</v>
+      </c>
+      <c r="E26">
+        <v>3.9260128886416432E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>500</v>
+      </c>
+      <c r="C27">
+        <v>500</v>
+      </c>
+      <c r="D27">
+        <v>0.21399261309946926</v>
+      </c>
+      <c r="E27">
+        <v>3.575899448291351E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>95</v>
+      </c>
+      <c r="C28">
+        <v>100</v>
+      </c>
+      <c r="D28">
+        <v>0.65210190965986004</v>
+      </c>
+      <c r="E28">
+        <v>2.3525299252587884E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>145</v>
+      </c>
+      <c r="C29">
+        <v>150</v>
+      </c>
+      <c r="D29">
+        <v>0.40268482863168548</v>
+      </c>
+      <c r="E29">
+        <v>2.9745489343523987E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>195</v>
+      </c>
+      <c r="C30">
+        <v>200</v>
+      </c>
+      <c r="D30">
+        <v>0.34040161624669435</v>
+      </c>
+      <c r="E30">
+        <v>3.6808070601383025E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>330</v>
+      </c>
+      <c r="C31">
+        <v>330</v>
+      </c>
+      <c r="D31">
+        <v>0.21967390507816151</v>
+      </c>
+      <c r="E31">
+        <v>2.5426631566395991E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <v>500</v>
+      </c>
+      <c r="C32">
+        <v>500</v>
+      </c>
+      <c r="D32">
+        <v>0.15443852951405687</v>
+      </c>
+      <c r="E32">
+        <v>3.8273754905766372E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>7</v>
+      </c>
+      <c r="B33">
+        <v>50</v>
+      </c>
+      <c r="C33">
+        <v>50</v>
+      </c>
+      <c r="D33">
+        <v>2.0862322401055753</v>
+      </c>
+      <c r="E33">
+        <v>0.12257369120655047</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34">
+        <v>95</v>
+      </c>
+      <c r="C34">
+        <v>100</v>
+      </c>
+      <c r="D34">
+        <v>0.82699046771144313</v>
+      </c>
+      <c r="E34">
+        <v>6.7066488403314528E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>7</v>
+      </c>
+      <c r="B35">
+        <v>145</v>
+      </c>
+      <c r="C35">
+        <v>150</v>
+      </c>
+      <c r="D35">
+        <v>0.4914583239158094</v>
+      </c>
+      <c r="E35">
+        <v>4.7291934361336718E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>7</v>
+      </c>
+      <c r="B36">
+        <v>195</v>
+      </c>
+      <c r="C36">
+        <v>200</v>
+      </c>
+      <c r="D36">
+        <v>0.35944956127142574</v>
+      </c>
+      <c r="E36">
+        <v>4.922273949119884E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>7</v>
+      </c>
+      <c r="B37">
+        <v>330</v>
+      </c>
+      <c r="C37">
+        <v>330</v>
+      </c>
+      <c r="D37">
+        <v>0.21406552933849277</v>
+      </c>
+      <c r="E37">
+        <v>3.7923870876550247E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38">
+        <v>500</v>
+      </c>
+      <c r="C38">
+        <v>500</v>
+      </c>
+      <c r="D38">
+        <v>0.15771459575203445</v>
+      </c>
+      <c r="E38">
+        <v>2.6115791303377347E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>20</v>
+      </c>
+      <c r="C39">
+        <v>30</v>
+      </c>
+      <c r="D39">
+        <v>2.1335809620681485</v>
+      </c>
+      <c r="E39">
+        <v>0.11083333333333334</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>8</v>
+      </c>
+      <c r="B40">
+        <v>50</v>
+      </c>
+      <c r="C40">
+        <v>50</v>
+      </c>
+      <c r="D40">
+        <v>0.9758014725638281</v>
+      </c>
+      <c r="E40">
+        <v>3.3867328232072669E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>8</v>
+      </c>
+      <c r="B41">
+        <v>95</v>
+      </c>
+      <c r="C41">
+        <v>100</v>
+      </c>
+      <c r="D41">
+        <v>0.64734010628759597</v>
+      </c>
+      <c r="E41">
+        <v>2.6218901136227619E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>8</v>
+      </c>
+      <c r="B42">
+        <v>145</v>
+      </c>
+      <c r="C42">
+        <v>150</v>
+      </c>
+      <c r="D42">
+        <v>0.35063138432344926</v>
+      </c>
+      <c r="E42">
+        <v>1.8502702691833513E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>8</v>
+      </c>
+      <c r="B43">
+        <v>195</v>
+      </c>
+      <c r="C43">
+        <v>200</v>
+      </c>
+      <c r="D43">
+        <v>0.31614042201083586</v>
+      </c>
+      <c r="E43">
+        <v>2.8996617768341684E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44">
+        <v>330</v>
+      </c>
+      <c r="C44">
+        <v>330</v>
+      </c>
+      <c r="D44">
+        <v>0.21353061336959622</v>
+      </c>
+      <c r="E44">
+        <v>3.6695666878826083E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>500</v>
+      </c>
+      <c r="C45">
+        <v>500</v>
+      </c>
+      <c r="D45">
+        <v>0.15309451285970466</v>
+      </c>
+      <c r="E45">
+        <v>1.589677511146538E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>9</v>
+      </c>
+      <c r="B46">
+        <v>50</v>
+      </c>
+      <c r="C46">
+        <v>50</v>
+      </c>
+      <c r="D46">
+        <v>1.8889306706365374</v>
+      </c>
+      <c r="E46">
+        <v>5.2446558986196719E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>9</v>
+      </c>
+      <c r="B47">
+        <v>105</v>
+      </c>
+      <c r="C47">
+        <v>100</v>
+      </c>
+      <c r="D47">
+        <v>0.68986024117012812</v>
+      </c>
+      <c r="E47">
+        <v>4.6007325240254589E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>9</v>
+      </c>
+      <c r="B48">
+        <v>155</v>
+      </c>
+      <c r="C48">
+        <v>150</v>
+      </c>
+      <c r="D48">
+        <v>0.41012689716507217</v>
+      </c>
+      <c r="E48">
+        <v>2.8084778950115907E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>9</v>
+      </c>
+      <c r="B49">
+        <v>205</v>
+      </c>
+      <c r="C49">
+        <v>200</v>
+      </c>
+      <c r="D49">
+        <v>0.34930412292010909</v>
+      </c>
+      <c r="E49">
+        <v>3.9328772375380364E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>9</v>
+      </c>
+      <c r="B50">
+        <v>330</v>
+      </c>
+      <c r="C50">
+        <v>330</v>
+      </c>
+      <c r="D50">
+        <v>0.24185242174902311</v>
+      </c>
+      <c r="E50">
+        <v>4.2415997614430399E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>9</v>
+      </c>
+      <c r="B51">
+        <v>500</v>
+      </c>
+      <c r="C51">
+        <v>500</v>
+      </c>
+      <c r="D51">
+        <v>0.16507143058586721</v>
+      </c>
+      <c r="E51">
+        <v>2.4669024309402304E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>10</v>
+      </c>
+      <c r="B52">
+        <v>105</v>
+      </c>
+      <c r="C52">
+        <v>100</v>
+      </c>
+      <c r="D52">
+        <v>0.61268369080156793</v>
+      </c>
+      <c r="E52">
+        <v>5.4068029604193102E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>10</v>
+      </c>
+      <c r="B53">
+        <v>155</v>
+      </c>
+      <c r="C53">
+        <v>150</v>
+      </c>
+      <c r="D53">
+        <v>0.41840792136671229</v>
+      </c>
+      <c r="E53">
+        <v>2.9290822851133134E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>10</v>
+      </c>
+      <c r="B54">
+        <v>500</v>
+      </c>
+      <c r="C54">
+        <v>500</v>
+      </c>
+      <c r="D54">
+        <v>0.17051274415014003</v>
+      </c>
+      <c r="E54">
+        <v>1.8834443789705602E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>11</v>
+      </c>
+      <c r="B55">
+        <v>50</v>
+      </c>
+      <c r="C55">
+        <v>50</v>
+      </c>
+      <c r="D55">
+        <v>1.7508734449029284</v>
+      </c>
+      <c r="E55">
+        <v>0.13598873559907138</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>11</v>
+      </c>
+      <c r="B56">
+        <v>105</v>
+      </c>
+      <c r="C56">
+        <v>100</v>
+      </c>
+      <c r="D56">
+        <v>0.93090543398081349</v>
+      </c>
+      <c r="E56">
+        <v>4.9462824772530743E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>11</v>
+      </c>
+      <c r="B57">
+        <v>155</v>
+      </c>
+      <c r="C57">
+        <v>150</v>
+      </c>
+      <c r="D57">
+        <v>0.43478931621211175</v>
+      </c>
+      <c r="E57">
+        <v>3.6017266520729806E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>11</v>
+      </c>
+      <c r="B58">
+        <v>205</v>
+      </c>
+      <c r="C58">
+        <v>200</v>
+      </c>
+      <c r="D58">
+        <v>0.37532905938678524</v>
+      </c>
+      <c r="E58">
+        <v>2.6239280901594709E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>11</v>
+      </c>
+      <c r="B59">
+        <v>330</v>
+      </c>
+      <c r="C59">
+        <v>330</v>
+      </c>
+      <c r="D59">
+        <v>0.24992114090170844</v>
+      </c>
+      <c r="E59">
+        <v>2.1761460089424794E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>11</v>
+      </c>
+      <c r="B60">
+        <v>500</v>
+      </c>
+      <c r="C60">
+        <v>500</v>
+      </c>
+      <c r="D60">
+        <v>0.16363760626744964</v>
+      </c>
+      <c r="E60">
+        <v>2.2586520412806326E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>12</v>
+      </c>
+      <c r="B61">
+        <v>20</v>
+      </c>
+      <c r="C61">
+        <v>30</v>
+      </c>
+      <c r="D61">
+        <v>3.0134745290850256</v>
+      </c>
+      <c r="E61">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>12</v>
+      </c>
+      <c r="B62">
+        <v>50</v>
+      </c>
+      <c r="C62">
+        <v>50</v>
+      </c>
+      <c r="D62">
+        <v>1.9028142836262878</v>
+      </c>
+      <c r="E62">
+        <v>8.9637055493137816E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>12</v>
+      </c>
+      <c r="B63">
+        <v>105</v>
+      </c>
+      <c r="C63">
+        <v>100</v>
+      </c>
+      <c r="D63">
+        <v>0.69325873604742627</v>
+      </c>
+      <c r="E63">
+        <v>4.2202584596898705E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>12</v>
+      </c>
+      <c r="B64">
+        <v>155</v>
+      </c>
+      <c r="C64">
+        <v>150</v>
+      </c>
+      <c r="D64">
+        <v>0.41346647285293692</v>
+      </c>
+      <c r="E64">
+        <v>2.6346264992603636E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>12</v>
+      </c>
+      <c r="B65">
+        <v>205</v>
+      </c>
+      <c r="C65">
+        <v>200</v>
+      </c>
+      <c r="D65">
+        <v>0.33528738791980256</v>
+      </c>
+      <c r="E65">
+        <v>3.0759006894829171E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>12</v>
+      </c>
+      <c r="B66">
+        <v>500</v>
+      </c>
+      <c r="C66">
+        <v>500</v>
+      </c>
+      <c r="D66">
+        <v>0.15204253170455087</v>
+      </c>
+      <c r="E66">
+        <v>2.2952744734381036E-2</v>
       </c>
     </row>
   </sheetData>
@@ -707,1143 +1609,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE25169-79B8-4E46-8D5E-6F3E6298BD3C}">
-  <dimension ref="A1:E66"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>50</v>
-      </c>
-      <c r="C2">
-        <v>50</v>
-      </c>
-      <c r="D2">
-        <v>0.89018926324458014</v>
-      </c>
-      <c r="E2">
-        <v>5.1705846886633579E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>95</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3">
-        <v>0.7153182801862531</v>
-      </c>
-      <c r="E3">
-        <v>5.6390084453433444E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>145</v>
-      </c>
-      <c r="C4">
-        <v>150</v>
-      </c>
-      <c r="D4">
-        <v>0.45001749959423903</v>
-      </c>
-      <c r="E4">
-        <v>2.9521695366396945E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>195</v>
-      </c>
-      <c r="C5">
-        <v>200</v>
-      </c>
-      <c r="D5">
-        <v>0.32799509976152702</v>
-      </c>
-      <c r="E5">
-        <v>3.3186393281012902E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>330</v>
-      </c>
-      <c r="C6">
-        <v>330</v>
-      </c>
-      <c r="D6">
-        <v>0.23470265158527037</v>
-      </c>
-      <c r="E6">
-        <v>1.3346149733508459E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>500</v>
-      </c>
-      <c r="C7">
-        <v>500</v>
-      </c>
-      <c r="D7">
-        <v>0.16060151501673745</v>
-      </c>
-      <c r="E7">
-        <v>2.9017651343523899E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>95</v>
-      </c>
-      <c r="C8">
-        <v>100</v>
-      </c>
-      <c r="D8">
-        <v>0.76714065045124069</v>
-      </c>
-      <c r="E8">
-        <v>6.7528084284768516E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>145</v>
-      </c>
-      <c r="C9">
-        <v>150</v>
-      </c>
-      <c r="D9">
-        <v>0.45829556808001809</v>
-      </c>
-      <c r="E9">
-        <v>5.4768237017384015E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>195</v>
-      </c>
-      <c r="C10">
-        <v>200</v>
-      </c>
-      <c r="D10">
-        <v>0.36324594343047573</v>
-      </c>
-      <c r="E10">
-        <v>8.6819214292885818E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>330</v>
-      </c>
-      <c r="C11">
-        <v>330</v>
-      </c>
-      <c r="D11">
-        <v>0.26489067375352698</v>
-      </c>
-      <c r="E11">
-        <v>4.7020009797597462E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>500</v>
-      </c>
-      <c r="C12">
-        <v>500</v>
-      </c>
-      <c r="D12">
-        <v>0.17589614981315357</v>
-      </c>
-      <c r="E12">
-        <v>3.0020056295142577E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>3</v>
-      </c>
-      <c r="B13">
-        <v>50</v>
-      </c>
-      <c r="C13">
-        <v>50</v>
-      </c>
-      <c r="D13">
-        <v>1.2689791897719822</v>
-      </c>
-      <c r="E13">
-        <v>4.5664085135654703E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>3</v>
-      </c>
-      <c r="B14">
-        <v>95</v>
-      </c>
-      <c r="C14">
-        <v>100</v>
-      </c>
-      <c r="D14">
-        <v>0.60800985133817231</v>
-      </c>
-      <c r="E14">
-        <v>3.1485506684334891E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>3</v>
-      </c>
-      <c r="B15">
-        <v>330</v>
-      </c>
-      <c r="C15">
-        <v>330</v>
-      </c>
-      <c r="D15">
-        <v>0.2316044991594198</v>
-      </c>
-      <c r="E15">
-        <v>3.28077591613158E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>3</v>
-      </c>
-      <c r="B16">
-        <v>500</v>
-      </c>
-      <c r="C16">
-        <v>500</v>
-      </c>
-      <c r="D16">
-        <v>0.16308334946888314</v>
-      </c>
-      <c r="E16">
-        <v>2.8194862359707629E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>4</v>
-      </c>
-      <c r="B17">
-        <v>50</v>
-      </c>
-      <c r="C17">
-        <v>50</v>
-      </c>
-      <c r="D17">
-        <v>1.9210846893753761</v>
-      </c>
-      <c r="E17">
-        <v>5.629286089011809E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>4</v>
-      </c>
-      <c r="B18">
-        <v>95</v>
-      </c>
-      <c r="C18">
-        <v>100</v>
-      </c>
-      <c r="D18">
-        <v>0.68365844702112921</v>
-      </c>
-      <c r="E18">
-        <v>3.0527088383164643E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>4</v>
-      </c>
-      <c r="B19">
-        <v>145</v>
-      </c>
-      <c r="C19">
-        <v>150</v>
-      </c>
-      <c r="D19">
-        <v>0.30309983851927552</v>
-      </c>
-      <c r="E19">
-        <v>1.4723993683688132E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>4</v>
-      </c>
-      <c r="B20">
-        <v>195</v>
-      </c>
-      <c r="C20">
-        <v>200</v>
-      </c>
-      <c r="D20">
-        <v>0.20886446167605854</v>
-      </c>
-      <c r="E20">
-        <v>3.3939938719133519E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>4</v>
-      </c>
-      <c r="B21">
-        <v>330</v>
-      </c>
-      <c r="C21">
-        <v>330</v>
-      </c>
-      <c r="D21">
-        <v>0.23590323149316275</v>
-      </c>
-      <c r="E21">
-        <v>4.7415563866089437E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>4</v>
-      </c>
-      <c r="B22">
-        <v>500</v>
-      </c>
-      <c r="C22">
-        <v>500</v>
-      </c>
-      <c r="D22">
-        <v>0.14285656260224014</v>
-      </c>
-      <c r="E22">
-        <v>3.0217055848894739E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>5</v>
-      </c>
-      <c r="B23">
-        <v>50</v>
-      </c>
-      <c r="C23">
-        <v>50</v>
-      </c>
-      <c r="D23">
-        <v>1.0748191044702937</v>
-      </c>
-      <c r="E23">
-        <v>2.5844200517237025E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>5</v>
-      </c>
-      <c r="B24">
-        <v>95</v>
-      </c>
-      <c r="C24">
-        <v>100</v>
-      </c>
-      <c r="D24">
-        <v>0.61992127892280602</v>
-      </c>
-      <c r="E24">
-        <v>1.5874341595665566E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>5</v>
-      </c>
-      <c r="B25">
-        <v>145</v>
-      </c>
-      <c r="C25">
-        <v>150</v>
-      </c>
-      <c r="D25">
-        <v>0.35753418573162649</v>
-      </c>
-      <c r="E25">
-        <v>2.260660010593386E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>5</v>
-      </c>
-      <c r="B26">
-        <v>330</v>
-      </c>
-      <c r="C26">
-        <v>330</v>
-      </c>
-      <c r="D26">
-        <v>0.26901829959445928</v>
-      </c>
-      <c r="E26">
-        <v>3.9260128886416432E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>5</v>
-      </c>
-      <c r="B27">
-        <v>500</v>
-      </c>
-      <c r="C27">
-        <v>500</v>
-      </c>
-      <c r="D27">
-        <v>0.21399261309946926</v>
-      </c>
-      <c r="E27">
-        <v>3.575899448291351E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>6</v>
-      </c>
-      <c r="B28">
-        <v>95</v>
-      </c>
-      <c r="C28">
-        <v>100</v>
-      </c>
-      <c r="D28">
-        <v>0.65210190965986004</v>
-      </c>
-      <c r="E28">
-        <v>2.3525299252587884E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>6</v>
-      </c>
-      <c r="B29">
-        <v>145</v>
-      </c>
-      <c r="C29">
-        <v>150</v>
-      </c>
-      <c r="D29">
-        <v>0.40268482863168548</v>
-      </c>
-      <c r="E29">
-        <v>2.9745489343523987E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>6</v>
-      </c>
-      <c r="B30">
-        <v>195</v>
-      </c>
-      <c r="C30">
-        <v>200</v>
-      </c>
-      <c r="D30">
-        <v>0.34040161624669435</v>
-      </c>
-      <c r="E30">
-        <v>3.6808070601383025E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>6</v>
-      </c>
-      <c r="B31">
-        <v>330</v>
-      </c>
-      <c r="C31">
-        <v>330</v>
-      </c>
-      <c r="D31">
-        <v>0.21967390507816151</v>
-      </c>
-      <c r="E31">
-        <v>2.5426631566395991E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>6</v>
-      </c>
-      <c r="B32">
-        <v>500</v>
-      </c>
-      <c r="C32">
-        <v>500</v>
-      </c>
-      <c r="D32">
-        <v>0.15443852951405687</v>
-      </c>
-      <c r="E32">
-        <v>3.8273754905766372E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>7</v>
-      </c>
-      <c r="B33">
-        <v>50</v>
-      </c>
-      <c r="C33">
-        <v>50</v>
-      </c>
-      <c r="D33">
-        <v>2.0862322401055753</v>
-      </c>
-      <c r="E33">
-        <v>0.12257369120655047</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>7</v>
-      </c>
-      <c r="B34">
-        <v>95</v>
-      </c>
-      <c r="C34">
-        <v>100</v>
-      </c>
-      <c r="D34">
-        <v>0.82699046771144313</v>
-      </c>
-      <c r="E34">
-        <v>6.7066488403314528E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>7</v>
-      </c>
-      <c r="B35">
-        <v>145</v>
-      </c>
-      <c r="C35">
-        <v>150</v>
-      </c>
-      <c r="D35">
-        <v>0.4914583239158094</v>
-      </c>
-      <c r="E35">
-        <v>4.7291934361336718E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>7</v>
-      </c>
-      <c r="B36">
-        <v>195</v>
-      </c>
-      <c r="C36">
-        <v>200</v>
-      </c>
-      <c r="D36">
-        <v>0.35944956127142574</v>
-      </c>
-      <c r="E36">
-        <v>4.922273949119884E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>7</v>
-      </c>
-      <c r="B37">
-        <v>330</v>
-      </c>
-      <c r="C37">
-        <v>330</v>
-      </c>
-      <c r="D37">
-        <v>0.21406552933849277</v>
-      </c>
-      <c r="E37">
-        <v>3.7923870876550247E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>7</v>
-      </c>
-      <c r="B38">
-        <v>500</v>
-      </c>
-      <c r="C38">
-        <v>500</v>
-      </c>
-      <c r="D38">
-        <v>0.15771459575203445</v>
-      </c>
-      <c r="E38">
-        <v>2.6115791303377347E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>8</v>
-      </c>
-      <c r="B39">
-        <v>20</v>
-      </c>
-      <c r="C39">
-        <v>30</v>
-      </c>
-      <c r="D39">
-        <v>2.1335809620681485</v>
-      </c>
-      <c r="E39">
-        <v>0.11083333333333334</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>8</v>
-      </c>
-      <c r="B40">
-        <v>50</v>
-      </c>
-      <c r="C40">
-        <v>50</v>
-      </c>
-      <c r="D40">
-        <v>0.9758014725638281</v>
-      </c>
-      <c r="E40">
-        <v>3.3867328232072669E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>8</v>
-      </c>
-      <c r="B41">
-        <v>95</v>
-      </c>
-      <c r="C41">
-        <v>100</v>
-      </c>
-      <c r="D41">
-        <v>0.64734010628759597</v>
-      </c>
-      <c r="E41">
-        <v>2.6218901136227619E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>8</v>
-      </c>
-      <c r="B42">
-        <v>145</v>
-      </c>
-      <c r="C42">
-        <v>150</v>
-      </c>
-      <c r="D42">
-        <v>0.35063138432344926</v>
-      </c>
-      <c r="E42">
-        <v>1.8502702691833513E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>8</v>
-      </c>
-      <c r="B43">
-        <v>195</v>
-      </c>
-      <c r="C43">
-        <v>200</v>
-      </c>
-      <c r="D43">
-        <v>0.31614042201083586</v>
-      </c>
-      <c r="E43">
-        <v>2.8996617768341684E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>8</v>
-      </c>
-      <c r="B44">
-        <v>330</v>
-      </c>
-      <c r="C44">
-        <v>330</v>
-      </c>
-      <c r="D44">
-        <v>0.21353061336959622</v>
-      </c>
-      <c r="E44">
-        <v>3.6695666878826083E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>8</v>
-      </c>
-      <c r="B45">
-        <v>500</v>
-      </c>
-      <c r="C45">
-        <v>500</v>
-      </c>
-      <c r="D45">
-        <v>0.15309451285970466</v>
-      </c>
-      <c r="E45">
-        <v>1.589677511146538E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>9</v>
-      </c>
-      <c r="B46">
-        <v>50</v>
-      </c>
-      <c r="C46">
-        <v>50</v>
-      </c>
-      <c r="D46">
-        <v>1.8889306706365374</v>
-      </c>
-      <c r="E46">
-        <v>5.2446558986196719E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>9</v>
-      </c>
-      <c r="B47">
-        <v>105</v>
-      </c>
-      <c r="C47">
-        <v>100</v>
-      </c>
-      <c r="D47">
-        <v>0.68986024117012812</v>
-      </c>
-      <c r="E47">
-        <v>4.6007325240254589E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>9</v>
-      </c>
-      <c r="B48">
-        <v>155</v>
-      </c>
-      <c r="C48">
-        <v>150</v>
-      </c>
-      <c r="D48">
-        <v>0.41012689716507217</v>
-      </c>
-      <c r="E48">
-        <v>2.8084778950115907E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>9</v>
-      </c>
-      <c r="B49">
-        <v>205</v>
-      </c>
-      <c r="C49">
-        <v>200</v>
-      </c>
-      <c r="D49">
-        <v>0.34930412292010909</v>
-      </c>
-      <c r="E49">
-        <v>3.9328772375380364E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>9</v>
-      </c>
-      <c r="B50">
-        <v>330</v>
-      </c>
-      <c r="C50">
-        <v>330</v>
-      </c>
-      <c r="D50">
-        <v>0.24185242174902311</v>
-      </c>
-      <c r="E50">
-        <v>4.2415997614430399E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>9</v>
-      </c>
-      <c r="B51">
-        <v>500</v>
-      </c>
-      <c r="C51">
-        <v>500</v>
-      </c>
-      <c r="D51">
-        <v>0.16507143058586721</v>
-      </c>
-      <c r="E51">
-        <v>2.4669024309402304E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>10</v>
-      </c>
-      <c r="B52">
-        <v>105</v>
-      </c>
-      <c r="C52">
-        <v>100</v>
-      </c>
-      <c r="D52">
-        <v>0.61268369080156793</v>
-      </c>
-      <c r="E52">
-        <v>5.4068029604193102E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>10</v>
-      </c>
-      <c r="B53">
-        <v>155</v>
-      </c>
-      <c r="C53">
-        <v>150</v>
-      </c>
-      <c r="D53">
-        <v>0.41840792136671229</v>
-      </c>
-      <c r="E53">
-        <v>2.9290822851133134E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>10</v>
-      </c>
-      <c r="B54">
-        <v>500</v>
-      </c>
-      <c r="C54">
-        <v>500</v>
-      </c>
-      <c r="D54">
-        <v>0.17051274415014003</v>
-      </c>
-      <c r="E54">
-        <v>1.8834443789705602E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>11</v>
-      </c>
-      <c r="B55">
-        <v>50</v>
-      </c>
-      <c r="C55">
-        <v>50</v>
-      </c>
-      <c r="D55">
-        <v>1.7508734449029284</v>
-      </c>
-      <c r="E55">
-        <v>0.13598873559907138</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>11</v>
-      </c>
-      <c r="B56">
-        <v>105</v>
-      </c>
-      <c r="C56">
-        <v>100</v>
-      </c>
-      <c r="D56">
-        <v>0.93090543398081349</v>
-      </c>
-      <c r="E56">
-        <v>4.9462824772530743E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>11</v>
-      </c>
-      <c r="B57">
-        <v>155</v>
-      </c>
-      <c r="C57">
-        <v>150</v>
-      </c>
-      <c r="D57">
-        <v>0.43478931621211175</v>
-      </c>
-      <c r="E57">
-        <v>3.6017266520729806E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>11</v>
-      </c>
-      <c r="B58">
-        <v>205</v>
-      </c>
-      <c r="C58">
-        <v>200</v>
-      </c>
-      <c r="D58">
-        <v>0.37532905938678524</v>
-      </c>
-      <c r="E58">
-        <v>2.6239280901594709E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>11</v>
-      </c>
-      <c r="B59">
-        <v>330</v>
-      </c>
-      <c r="C59">
-        <v>330</v>
-      </c>
-      <c r="D59">
-        <v>0.24992114090170844</v>
-      </c>
-      <c r="E59">
-        <v>2.1761460089424794E-2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>11</v>
-      </c>
-      <c r="B60">
-        <v>500</v>
-      </c>
-      <c r="C60">
-        <v>500</v>
-      </c>
-      <c r="D60">
-        <v>0.16363760626744964</v>
-      </c>
-      <c r="E60">
-        <v>2.2586520412806326E-2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>12</v>
-      </c>
-      <c r="B61">
-        <v>20</v>
-      </c>
-      <c r="C61">
-        <v>30</v>
-      </c>
-      <c r="D61">
-        <v>3.0134745290850256</v>
-      </c>
-      <c r="E61">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>12</v>
-      </c>
-      <c r="B62">
-        <v>50</v>
-      </c>
-      <c r="C62">
-        <v>50</v>
-      </c>
-      <c r="D62">
-        <v>1.9028142836262878</v>
-      </c>
-      <c r="E62">
-        <v>8.9637055493137816E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>12</v>
-      </c>
-      <c r="B63">
-        <v>105</v>
-      </c>
-      <c r="C63">
-        <v>100</v>
-      </c>
-      <c r="D63">
-        <v>0.69325873604742627</v>
-      </c>
-      <c r="E63">
-        <v>4.2202584596898705E-2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>12</v>
-      </c>
-      <c r="B64">
-        <v>155</v>
-      </c>
-      <c r="C64">
-        <v>150</v>
-      </c>
-      <c r="D64">
-        <v>0.41346647285293692</v>
-      </c>
-      <c r="E64">
-        <v>2.6346264992603636E-2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>12</v>
-      </c>
-      <c r="B65">
-        <v>205</v>
-      </c>
-      <c r="C65">
-        <v>200</v>
-      </c>
-      <c r="D65">
-        <v>0.33528738791980256</v>
-      </c>
-      <c r="E65">
-        <v>3.0759006894829171E-2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>12</v>
-      </c>
-      <c r="B66">
-        <v>500</v>
-      </c>
-      <c r="C66">
-        <v>500</v>
-      </c>
-      <c r="D66">
-        <v>0.15204253170455087</v>
-      </c>
-      <c r="E66">
-        <v>2.2952744734381036E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639A4B54-69C4-CD45-9C32-AD6199B4442F}">
   <dimension ref="A1:E66"/>
   <sheetViews>
@@ -1855,19 +1620,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2985,7 +2750,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D03F993A-AD12-D740-B288-3D4A4563011C}">
   <dimension ref="A1:E71"/>
   <sheetViews>
@@ -2997,19 +2762,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -4207,7 +3972,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CED31C6-DEAB-CD40-9B03-17A7DE5EE234}">
   <dimension ref="A1:D55"/>
   <sheetViews>
@@ -4219,21 +3984,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -4247,7 +4012,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -4261,7 +4026,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -4270,12 +4035,12 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>32</v>
@@ -4289,7 +4054,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>70</v>
@@ -4303,7 +4068,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -4317,7 +4082,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>8</v>
@@ -4331,7 +4096,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>20</v>
@@ -4340,12 +4105,12 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>32</v>
@@ -4359,7 +4124,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <v>70</v>
@@ -4373,7 +4138,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -4387,7 +4152,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B13">
         <v>8</v>
@@ -4401,7 +4166,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>20</v>
@@ -4410,12 +4175,12 @@
         <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B15">
         <v>32</v>
@@ -4429,7 +4194,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B16">
         <v>70</v>
@@ -4443,7 +4208,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -4457,7 +4222,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B18">
         <v>8</v>
@@ -4471,7 +4236,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <v>20</v>
@@ -4480,12 +4245,12 @@
         <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B20">
         <v>32</v>
@@ -4499,7 +4264,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B21">
         <v>70</v>
@@ -4513,7 +4278,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -4527,7 +4292,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -4541,7 +4306,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B24">
         <v>20</v>
@@ -4550,12 +4315,12 @@
         <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B25">
         <v>32</v>
@@ -4569,7 +4334,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B26">
         <v>70</v>
@@ -4583,7 +4348,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B27">
         <v>12</v>
@@ -4597,7 +4362,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B28">
         <v>12</v>
@@ -4611,7 +4376,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B29">
         <v>18</v>
@@ -4625,7 +4390,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B30">
         <v>28</v>
@@ -4639,7 +4404,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B31">
         <v>50</v>
@@ -4653,7 +4418,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B32">
         <v>68</v>
@@ -4667,7 +4432,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B33">
         <v>12</v>
@@ -4681,7 +4446,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B34">
         <v>12</v>
@@ -4695,7 +4460,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B35">
         <v>18</v>
@@ -4704,12 +4469,12 @@
         <v>20</v>
       </c>
       <c r="D35" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B36">
         <v>28</v>
@@ -4723,7 +4488,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B37">
         <v>50</v>
@@ -4737,7 +4502,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B38">
         <v>68</v>
@@ -4751,7 +4516,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B39">
         <v>12</v>
@@ -4765,7 +4530,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B40">
         <v>12</v>
@@ -4779,7 +4544,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B41">
         <v>18</v>
@@ -4793,7 +4558,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B42">
         <v>28</v>
@@ -4807,7 +4572,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B43">
         <v>50</v>
@@ -4821,7 +4586,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B44">
         <v>68</v>
@@ -4835,7 +4600,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B45">
         <v>3</v>
@@ -4849,7 +4614,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B46">
         <v>9</v>
@@ -4863,7 +4628,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B47">
         <v>19</v>
@@ -4877,7 +4642,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B48">
         <v>32</v>
@@ -4891,7 +4656,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B49">
         <v>67</v>
@@ -4905,7 +4670,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B50">
         <v>9</v>
@@ -4919,7 +4684,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B51">
         <v>9</v>
@@ -4933,7 +4698,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B52">
         <v>20</v>
@@ -4947,7 +4712,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B53">
         <v>31</v>
@@ -4961,7 +4726,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B54">
         <v>42</v>
@@ -4975,7 +4740,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B55">
         <v>67</v>
@@ -4992,11 +4757,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E83C3958-FCD0-504B-85EE-BABA48F3BBD1}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
@@ -5007,10 +4772,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -5128,7 +4893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D38FDAF-9FD7-B14F-9CC4-697685663D99}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -5143,10 +4908,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>